<commit_message>
feat: add help modals and improve requirement editing process
</commit_message>
<xml_diff>
--- a/uploads/modifications.xlsx
+++ b/uploads/modifications.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,10 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Detected Terms</t>
+          <t>Modified Requirement</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Edit Option</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Modified Requirement</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Original Requirement</t>
         </is>
@@ -458,20 +448,10 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>allow (Vague expressions), provide (Vague expressions), support (Vague expressions), potentially (Adverbs)</t>
+          <t>The CITIS must provide Canada with access to automated TPM processes, features, tools, and data to support Canada's responsibilities in the notification, tracking, and reporting of MHWS acquisition and in-service technical problems. The CITIS must potentially allow a user to initiate and log help requests relating to the Contractor-provided elements of the IIE and query their details, including the problem, the initiator, the owner, solutions tried, resolution, open/closed status, and response time.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
-        <is>
-          <t>Term Modification</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>The CITIS must provide Canada with access to automated TPM processes, features, tools, and data to support Canada's responsibilities in the notification, tracking, and reporting of MHWS acquisition and in-service technical problems. The CITIS must potentially allow a user to initiate and log help requests relating to the Contractor-provided elements of the IIE and query their details, including the problem, the initiator, the owner, solutions tried, resolution, open/closed status, and response time.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
         <is>
           <t>The CITIS must provide Canada with access to automated TPM processes, features, tools, and data to support Canada's responsibilities in the notification, tracking, and reporting of MHWS acquisition and in-service technical problems. The CITIS must potentially allow a user to initiate and log help requests relating to the Contractor-provided elements of the IIE and query their details, including the problem, the initiator, the owner, solutions tried, resolution, open/closed status, and response time.</t>
         </is>
@@ -480,20 +460,10 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>not (Vague expressions), allow (Vague expressions), expected (Vague expressions)</t>
+          <t>The ERMS must not allow a user to have access to classes, folders or records or their metadata (according to configuration) by means of any search and retrieval function, where the access controls and protective markings allocated to those classes, folders or records prevent access by that user. The ERMS is expected to be capable of supporting the integration, within the design arch</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
-        <is>
-          <t>Term Modification</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>The ERMS must eveveve eeveevev a user to have access to classes, folders or records or their metadata (according to configuration) by means of any search and retrieval function, where the access controls and protective markings allocated to those classes, folders or records prevent access by that user. The ERMS is evevv to be capable of supporting the integration, within the design arch</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
         <is>
           <t>The ERMS must not allow a user to have access to classes, folders or records or their metadata (according to configuration) by means of any search and retrieval function, where the access controls and protective markings allocated to those classes, folders or records prevent access by that user. The ERMS is expected to be capable of supporting the integration, within the design arch</t>
         </is>
@@ -502,20 +472,10 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>at (Vague expressions), may be (Vague expressions)</t>
+          <t>Computers used at the Gemini 8m Telescopes site, particularly in the test phase when they are outside the control room and near the subsystem under test, may be checked against altitude and humidity specifications for the Gemini 8m Telescopes site</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
-        <is>
-          <t>Term Modification</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Computers used eeeeeeee the Gemini 8m Telescopes site, particularly in the test phase when they are outside the control room and near the subsystem under test, may be checked against altitude and humidity specifications for the Gemini 8m Telescopes site</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>Computers used at the Gemini 8m Telescopes site, particularly in the test phase when they are outside the control room and near the subsystem under test, may be checked against altitude and humidity specifications for the Gemini 8m Telescopes site</t>
         </is>
@@ -524,20 +484,10 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>some (Unclear terms), may be (Vague expressions)</t>
+          <t>When a functional number change is required, the user may be able to initiate the change, store/retrieve numbers and some details.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
-        <is>
-          <t>Term Modification</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>When a functional number change is required, the user eeee able to initiate the change, store/retrieve numbers and eeeeeee details.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
         <is>
           <t>When a functional number change is required, the user may be able to initiate the change, store/retrieve numbers and some details.</t>
         </is>
@@ -546,20 +496,10 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>possibility (Vague expressions), ensure (Vague expressions), expected (Vague expressions), ideally (Adjectives)</t>
+          <t>The ERMS is ideally expected to ensure the possibility of providing a configurable option that defines how the access control mechanism operates. This ensures that either a user without the required permissions for a class, folder, or record is completely unaware of its existence or is explicitly notified of restricted access.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
-        <is>
-          <t>Term Modification</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>The ERMS is effefe efef to efefef the fefef of providing a configurable option that defines how the access control mechanism operates. This ensures that either a user without the required permissions for a class, folder, or record is completely unaware of its existence or is explicitly notified of restricted access.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
         <is>
           <t>The ERMS is ideally expected to ensure the possibility of providing a configurable option that defines how the access control mechanism operates. This ensures that either a user without the required permissions for a class, folder, or record is completely unaware of its existence or is explicitly notified of restricted access.</t>
         </is>
@@ -568,20 +508,10 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>may be (Vague expressions)</t>
+          <t>Only one database file is allowed in command line options. In case a space is found in the path, it may be enclosed into quotes</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
-        <is>
-          <t>Term Modification</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Only one database file is allowed in command line options. In case a space is found in the path, it fefef enclosed into quotes</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
         <is>
           <t>Only one database file is allowed in command line options. In case a space is found in the path, it may be enclosed into quotes</t>
         </is>
@@ -590,20 +520,10 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>other (Unclear terms), support (Vague expressions), may be (Vague expressions)</t>
+          <t>The TIMS will support the administration and management of the MH Training Program resources. It will support the allocation of resources and the monitoring of training delivery. This has the potential to include servers, PCs, laptops, tablets, PEDDs, or other external computing devices, as well as embedded computers. All computer devices used to support MH Training Program activities may be electronically compatible within its defined external electromagnetic environment.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
-        <is>
-          <t>Term Modification</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>The TIMS will support the administration and management of the MH Training Program resources. It will support the allocation of resources and the monitoring of training delivery. This has the potential to include servers, PCs, laptops, tablets, PEDDs, or other external computing devices, as well as embedded computers. All computer devices used to support MH Training Program activities may be electronically compatible within its defined external electromagnetic environment.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>The TIMS will support the administration and management of the MH Training Program resources. It will support the allocation of resources and the monitoring of training delivery. This has the potential to include servers, PCs, laptops, tablets, PEDDs, or other external computing devices, as well as embedded computers. All computer devices used to support MH Training Program activities may be electronically compatible within its defined external electromagnetic environment.</t>
         </is>
@@ -612,20 +532,10 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>not (Vague expressions), at (Vague expressions), expected (Vague expressions)</t>
+          <t>When creating a new electronic folder in a classification scheme which uses a structured numerical or alphanumerical reference, the ERMS is expected to automatically generate the next sequential number available at that position within the scheme. The ERMS must not, by its own architecture or design, impose any practical limit on the number of folders which can be created under any class, or within the entire ERMS.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
-        <is>
-          <t>Term Modification</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>When creating a new electronic folder in a classification scheme which uses a structured numerical or alphanumerical reference, the ERMS is efef to automatically generate the next sequential number available at that position within the scheme. The ERMS must efefe, by its own architecture or design, impose any practical limit on the number of folders which can be created under any class, or within the entire ERMS.</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
         <is>
           <t>When creating a new electronic folder in a classification scheme which uses a structured numerical or alphanumerical reference, the ERMS is expected to automatically generate the next sequential number available at that position within the scheme. The ERMS must not, by its own architecture or design, impose any practical limit on the number of folders which can be created under any class, or within the entire ERMS.</t>
         </is>

</xml_diff>